<commit_message>
Risk assessment spreadsheet updated as per meeting 8.1.19
</commit_message>
<xml_diff>
--- a/Development plans/Ship Happens - Risk Assessment Spreadsheet.xlsx
+++ b/Development plans/Ship Happens - Risk Assessment Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2133044E-9246-4888-8D44-A25C193C3FB3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ECB26454-1DF6-42FB-A8AA-268BDBFFD044}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
   <si>
     <t>Project Name</t>
   </si>
@@ -114,6 +113,9 @@
   </si>
   <si>
     <t>Develop for Console</t>
+  </si>
+  <si>
+    <t>Tutorial (intuitiveness)</t>
   </si>
 </sst>
 </file>
@@ -123,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +165,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -467,7 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -483,90 +491,90 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -575,6 +583,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -860,7 +871,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,58 +887,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="34" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="36"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="34" t="s">
+      <c r="B4" s="33"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
@@ -939,41 +950,41 @@
       </c>
       <c r="B5" s="38"/>
       <c r="C5" s="39"/>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="34"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="30" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="4"/>
@@ -982,30 +993,30 @@
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="33"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="31"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="23" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="1"/>
@@ -1014,11 +1025,11 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="8" t="s">
         <v>11</v>
       </c>
@@ -1034,11 +1045,11 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="8" t="s">
         <v>11</v>
       </c>
@@ -1054,11 +1065,11 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="8" t="s">
         <v>11</v>
       </c>
@@ -1074,11 +1085,11 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="8" t="s">
         <v>11</v>
       </c>
@@ -1094,11 +1105,11 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="8" t="s">
         <v>11</v>
       </c>
@@ -1114,18 +1125,18 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="21" t="s">
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G15" s="1"/>
@@ -1134,18 +1145,18 @@
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="21" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="1"/>
@@ -1154,18 +1165,18 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="22" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G17" s="1"/>
@@ -1174,18 +1185,18 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="22" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G18" s="1"/>
@@ -1194,11 +1205,11 @@
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="8" t="s">
         <v>11</v>
       </c>
@@ -1214,19 +1225,19 @@
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="21" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>19</v>
+      <c r="F20" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1234,13 +1245,13 @@
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="8" t="s">
-        <v>11</v>
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>11</v>
@@ -1254,18 +1265,18 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="22" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G22" s="1"/>
@@ -1274,11 +1285,11 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="17"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="8" t="s">
         <v>11</v>
       </c>
@@ -1294,11 +1305,11 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="17"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="8" t="s">
         <v>11</v>
       </c>
@@ -1314,12 +1325,12 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="22" t="s">
+      <c r="B25" s="13"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E25" s="8" t="s">
@@ -1334,21 +1345,29 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="A26" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="40" t="s">
+        <v>19</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -1358,9 +1377,9 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -1370,9 +1389,9 @@
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="17"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="14"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -1382,9 +1401,9 @@
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="17"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="14"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -1394,9 +1413,9 @@
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="17"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -1406,9 +1425,9 @@
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="17"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="14"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -1418,9 +1437,9 @@
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="17"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="14"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -1430,9 +1449,9 @@
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="14"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -1442,9 +1461,9 @@
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -1455,29 +1474,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A16:C16"/>
@@ -1487,14 +1491,29 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:C34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>